<commit_message>
Adding the adler32 hash function
</commit_message>
<xml_diff>
--- a/graphs/newCDC.xlsx
+++ b/graphs/newCDC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -222,14 +222,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1316,7 +1315,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1387,61 +1385,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>73.319198299643602</c:v>
+                  <c:v>50.737040595508503</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1240.32663095969</c:v>
+                  <c:v>87.698773863107206</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1254.3136210264599</c:v>
+                  <c:v>67.820918453081106</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1341.18965107999</c:v>
+                  <c:v>201.32371804007599</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1636.28865979381</c:v>
+                  <c:v>106.678749707363</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>164256.74418604601</c:v>
+                  <c:v>408.64614672529501</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2115.4743541744601</c:v>
+                  <c:v>258.95418007167598</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4973.0962858651601</c:v>
+                  <c:v>686.88240013614995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3621.6074862197102</c:v>
+                  <c:v>223.67318502097999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3081.2694950376199</c:v>
+                  <c:v>441.15738355116201</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1837.6583842851501</c:v>
+                  <c:v>124.219717987838</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4537.0419142444198</c:v>
+                  <c:v>158.18235771674901</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1284189.0909090899</c:v>
+                  <c:v>1028.36093619189</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3621.6074862197102</c:v>
+                  <c:v>305.88510426365798</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2156.9827454573201</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>14126080</c:v>
+                  <c:v>1745.2532740301399</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>805.93809727570897</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>88564.764890282095</c:v>
+                  <c:v>1813.36071887034</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4552.3944569771102</c:v>
+                  <c:v>473.39410187667499</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4552.3944569771102</c:v>
+                  <c:v>233.974277219687</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1453,61 +1451,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0.91247274544671897</c:v>
+                  <c:v>0.94417053421756003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.72688484703470402</c:v>
+                  <c:v>0.91433338194318503</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.71715943134967297</c:v>
+                  <c:v>0.930415904483055</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.59967298075616104</c:v>
+                  <c:v>0.89749176700117705</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.67201990927419297</c:v>
+                  <c:v>0.90972134519979997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.1729411131750598E-2</c:v>
+                  <c:v>0.86152106599990896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.62699198928506705</c:v>
+                  <c:v>0.88079838851259495</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.43109539235230099</c:v>
+                  <c:v>0.82217918913102495</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.47012171812703801</c:v>
+                  <c:v>0.89186189657711101</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.57501536165730305</c:v>
+                  <c:v>0.84738083742977499</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.64961408260465703</c:v>
+                  <c:v>0.90553267431587503</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.39654645874863997</c:v>
+                  <c:v>0.89525399119925697</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.9723929073033696E-3</c:v>
+                  <c:v>0.78186078515766499</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.47012171812703801</c:v>
+                  <c:v>0.86400873419943802</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.62256404466065596</c:v>
+                  <c:v>0.71798280202292497</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>0.81614641146022104</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.13098609097499E-2</c:v>
+                  <c:v>0.70777462678959702</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.39057406584133703</c:v>
+                  <c:v>0.84565020869200802</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.39057406584133703</c:v>
+                  <c:v>0.87836869818095298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1701,7 +1699,7 @@
         <c:axId val="338160896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="5000"/>
+          <c:max val="2000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1750,7 +1748,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1798,7 +1795,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1868,7 +1865,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1949,7 +1945,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2061,7 +2056,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2489,7 +2483,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2607,7 +2600,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2688,7 +2680,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2795,7 +2786,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3203,7 +3193,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3321,7 +3310,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3402,7 +3390,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3509,7 +3496,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3917,7 +3903,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4035,7 +4020,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4116,7 +4100,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7679,6 +7662,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -7714,6 +7714,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -10624,7 +10641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -11773,8 +11790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12233,10 +12250,10 @@
         <v>100</v>
       </c>
       <c r="B30">
-        <v>73.319198299643602</v>
+        <v>50.737040595508503</v>
       </c>
       <c r="C30">
-        <v>0.91247274544671897</v>
+        <v>0.94417053421756003</v>
       </c>
       <c r="D30">
         <v>100</v>
@@ -12253,10 +12270,10 @@
         <v>150</v>
       </c>
       <c r="B31">
-        <v>1240.32663095969</v>
+        <v>87.698773863107206</v>
       </c>
       <c r="C31">
-        <v>0.72688484703470402</v>
+        <v>0.91433338194318503</v>
       </c>
       <c r="D31">
         <v>150</v>
@@ -12273,10 +12290,10 @@
         <v>200</v>
       </c>
       <c r="B32">
-        <v>1254.3136210264599</v>
+        <v>67.820918453081106</v>
       </c>
       <c r="C32">
-        <v>0.71715943134967297</v>
+        <v>0.930415904483055</v>
       </c>
       <c r="D32">
         <v>200</v>
@@ -12293,10 +12310,10 @@
         <v>250</v>
       </c>
       <c r="B33">
-        <v>1341.18965107999</v>
+        <v>201.32371804007599</v>
       </c>
       <c r="C33">
-        <v>0.59967298075616104</v>
+        <v>0.89749176700117705</v>
       </c>
       <c r="D33">
         <v>250</v>
@@ -12313,10 +12330,10 @@
         <v>300</v>
       </c>
       <c r="B34">
-        <v>1636.28865979381</v>
+        <v>106.678749707363</v>
       </c>
       <c r="C34">
-        <v>0.67201990927419297</v>
+        <v>0.90972134519979997</v>
       </c>
       <c r="D34">
         <v>300</v>
@@ -12333,10 +12350,10 @@
         <v>350</v>
       </c>
       <c r="B35">
-        <v>164256.74418604601</v>
+        <v>408.64614672529501</v>
       </c>
       <c r="C35">
-        <v>4.1729411131750598E-2</v>
+        <v>0.86152106599990896</v>
       </c>
       <c r="D35">
         <v>350</v>
@@ -12353,10 +12370,10 @@
         <v>400</v>
       </c>
       <c r="B36">
-        <v>2115.4743541744601</v>
+        <v>258.95418007167598</v>
       </c>
       <c r="C36">
-        <v>0.62699198928506705</v>
+        <v>0.88079838851259495</v>
       </c>
       <c r="D36">
         <v>400</v>
@@ -12373,10 +12390,10 @@
         <v>450</v>
       </c>
       <c r="B37">
-        <v>4973.0962858651601</v>
+        <v>686.88240013614995</v>
       </c>
       <c r="C37">
-        <v>0.43109539235230099</v>
+        <v>0.82217918913102495</v>
       </c>
       <c r="D37">
         <v>450</v>
@@ -12393,10 +12410,10 @@
         <v>500</v>
       </c>
       <c r="B38">
-        <v>3621.6074862197102</v>
+        <v>223.67318502097999</v>
       </c>
       <c r="C38">
-        <v>0.47012171812703801</v>
+        <v>0.89186189657711101</v>
       </c>
       <c r="D38">
         <v>500</v>
@@ -12413,10 +12430,10 @@
         <v>550</v>
       </c>
       <c r="B39">
-        <v>3081.2694950376199</v>
+        <v>441.15738355116201</v>
       </c>
       <c r="C39">
-        <v>0.57501536165730305</v>
+        <v>0.84738083742977499</v>
       </c>
       <c r="D39">
         <v>550</v>
@@ -12433,10 +12450,10 @@
         <v>600</v>
       </c>
       <c r="B40">
-        <v>1837.6583842851501</v>
+        <v>124.219717987838</v>
       </c>
       <c r="C40">
-        <v>0.64961408260465703</v>
+        <v>0.90553267431587503</v>
       </c>
       <c r="D40">
         <v>600</v>
@@ -12453,10 +12470,10 @@
         <v>650</v>
       </c>
       <c r="B41">
-        <v>4537.0419142444198</v>
+        <v>158.18235771674901</v>
       </c>
       <c r="C41">
-        <v>0.39654645874863997</v>
+        <v>0.89525399119925697</v>
       </c>
       <c r="D41">
         <v>650</v>
@@ -12473,10 +12490,10 @@
         <v>700</v>
       </c>
       <c r="B42">
-        <v>1284189.0909090899</v>
+        <v>1028.36093619189</v>
       </c>
       <c r="C42">
-        <v>5.9723929073033696E-3</v>
+        <v>0.78186078515766499</v>
       </c>
       <c r="D42">
         <v>700</v>
@@ -12493,10 +12510,10 @@
         <v>750</v>
       </c>
       <c r="B43">
-        <v>3621.6074862197102</v>
+        <v>305.88510426365798</v>
       </c>
       <c r="C43">
-        <v>0.47012171812703801</v>
+        <v>0.86400873419943802</v>
       </c>
       <c r="D43">
         <v>750</v>
@@ -12513,10 +12530,10 @@
         <v>800</v>
       </c>
       <c r="B44">
-        <v>2156.9827454573201</v>
+        <v>1745.2532740301399</v>
       </c>
       <c r="C44">
-        <v>0.62256404466065596</v>
+        <v>0.71798280202292497</v>
       </c>
       <c r="D44">
         <v>800</v>
@@ -12532,11 +12549,11 @@
       <c r="A45">
         <v>850</v>
       </c>
-      <c r="B45" s="6">
-        <v>14126080</v>
+      <c r="B45">
+        <v>805.93809727570897</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>0.81614641146022104</v>
       </c>
       <c r="D45">
         <v>850</v>
@@ -12553,10 +12570,10 @@
         <v>900</v>
       </c>
       <c r="B46">
-        <v>88564.764890282095</v>
+        <v>1813.36071887034</v>
       </c>
       <c r="C46">
-        <v>1.13098609097499E-2</v>
+        <v>0.70777462678959702</v>
       </c>
       <c r="D46">
         <v>900</v>
@@ -12573,10 +12590,10 @@
         <v>950</v>
       </c>
       <c r="B47">
-        <v>4552.3944569771102</v>
+        <v>473.39410187667499</v>
       </c>
       <c r="C47">
-        <v>0.39057406584133703</v>
+        <v>0.84565020869200802</v>
       </c>
       <c r="D47">
         <v>950</v>
@@ -12593,10 +12610,10 @@
         <v>1000</v>
       </c>
       <c r="B48">
-        <v>4552.3944569771102</v>
+        <v>233.974277219687</v>
       </c>
       <c r="C48">
-        <v>0.39057406584133703</v>
+        <v>0.87836869818095298</v>
       </c>
       <c r="D48">
         <v>1000</v>

</xml_diff>